<commit_message>
Comitting all changes with errors 10/4/2022
</commit_message>
<xml_diff>
--- a/CustomQueueManager/Data/Config.xlsx
+++ b/CustomQueueManager/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexandra.veizu\Documents\Reframework_update_UiPath_Services\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Documents\UiPath\Custom_REFramework_Template\CustomQueueManager\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE7DFF5-5AFC-4110-8461-609B0BDD5551}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45259B2-2F3E-4AB1-94F0-0A63C19A1D37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2115" yWindow="600" windowWidth="21600" windowHeight="13995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -90,10 +90,6 @@
     <t>Framework</t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -122,6 +118,9 @@
   </si>
   <si>
     <t>OrchestratorAssetFolder</t>
+  </si>
+  <si>
+    <t>ProcessABCQueue</t>
   </si>
 </sst>
 </file>
@@ -499,8 +498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -547,13 +546,13 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -565,7 +564,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1624,7 +1623,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1648,7 +1647,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -1670,7 +1669,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -1681,7 +1680,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1692,7 +1691,7 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2682,7 +2681,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
@@ -2702,7 +2701,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>